<commit_message>
cập nhật ip planning queens
</commit_message>
<xml_diff>
--- a/tools/HCD_IP-Planning-Hardware-Requirements.xlsx
+++ b/tools/HCD_IP-Planning-Hardware-Requirements.xlsx
@@ -714,7 +714,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -751,12 +751,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color rgb="FFFF0000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="13"/>
       <color rgb="FFFF0000"/>
       <name val="Tahoma"/>
@@ -960,7 +954,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1271,9 +1265,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1562,7 +1553,7 @@
   <dimension ref="B2:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:F6"/>
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -1699,7 +1690,7 @@
       <c r="E6" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="106" t="s">
+      <c r="F6" s="51" t="s">
         <v>190</v>
       </c>
       <c r="G6" s="44" t="s">
@@ -1979,7 +1970,7 @@
         <v>26</v>
       </c>
       <c r="F15" s="46" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G15" s="44" t="s">
         <v>223</v>
@@ -2006,7 +1997,7 @@
         <v>34</v>
       </c>
       <c r="F16" s="47" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G16" s="44" t="s">
         <v>223</v>
@@ -2370,11 +2361,6 @@
     <mergeCell ref="P10:P13"/>
     <mergeCell ref="O14:O17"/>
     <mergeCell ref="P14:P17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="K18:K20"/>
-    <mergeCell ref="L18:L20"/>
-    <mergeCell ref="M18:M20"/>
     <mergeCell ref="N18:N20"/>
     <mergeCell ref="O18:O20"/>
     <mergeCell ref="P18:P20"/>
@@ -2384,6 +2370,11 @@
     <mergeCell ref="L14:L17"/>
     <mergeCell ref="M14:M17"/>
     <mergeCell ref="N14:N17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="L18:L20"/>
+    <mergeCell ref="M18:M20"/>
     <mergeCell ref="O21:O23"/>
     <mergeCell ref="P21:P23"/>
     <mergeCell ref="B24:B26"/>

</xml_diff>